<commit_message>
Merged in issue#155-2 (pull request #135)
issue #155 - translate R{key} in Excel template for national language support

* issue #155 - translate R{key} in Excel template for national language

    support

* issue #155 - translate R{key} in Excel template for national language

    support

* issue #155 - translate R{key} in Excel template for national language

    support

* issue #155 - translate R{key} in Excel template for national language

    support

* issue #155 - translate R{key} in Excel template for national language

    support

* issue #155 - translate R{key} in Excel template for national language

    support

Approved-by: LeonidV <leonate@gmail.com>
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls/templatebasedtests/PivotTableTest.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls/templatebasedtests/PivotTableTest.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\git-repos\jxls2-eclipse-2019-03\jxls-poi\src\test\resources\org\jxls\transform\poi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\warm\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2BF6F9-6FA6-421E-BA4A-A6D3D3F8F802}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B41AD6DD-EC40-4CA3-9DF7-6D5DE630AEDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{827B221D-7995-4EFA-A5B1-BD072CB58E18}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8B8F0785-C78F-4DD0-AFEA-8E0A4BB39FFB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table" sheetId="2" r:id="rId1"/>
-    <sheet name="PivotTable" sheetId="3" r:id="rId2"/>
+    <sheet name="Employees" sheetId="1" r:id="rId1"/>
+    <sheet name="Crosstab" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,6 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +40,7 @@
     <author>Marcus Warm</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{F92902D9-87B0-44EA-85B8-34B2788BFE4F}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{6B063B43-15D3-4DF8-9376-06F555A66FEC}">
       <text>
         <r>
           <rPr>
@@ -49,7 +50,7 @@
             <rFont val="Segoe UI"/>
             <charset val="1"/>
           </rPr>
-          <t>Marcus Warm:</t>
+          <t>JXLS team:</t>
         </r>
         <r>
           <rPr>
@@ -59,11 +60,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="B2")</t>
+jx:area(lastCell="C2")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{EC0A795D-EF2C-4120-BF1A-F113F73DAF88}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{8B43E323-CD6A-4956-9626-F2D56DF66604}">
       <text>
         <r>
           <rPr>
@@ -73,7 +74,7 @@
             <rFont val="Segoe UI"/>
             <charset val="1"/>
           </rPr>
-          <t>Marcus Warm:</t>
+          <t>JXLS team:</t>
         </r>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="list", var="a", lastCell="B2")</t>
+jx:each(items="employees", var="e", lastCell="C2")</t>
         </r>
       </text>
     </comment>
@@ -91,19 +92,59 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Marcus Warm</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{51585606-B67D-4292-82CA-FC41B15DC4FF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>JXLS team:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="A1")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>${a.name}</t>
-  </si>
-  <si>
-    <t>${a.city}</t>
-  </si>
-  <si>
-    <t>${R.name}</t>
-  </si>
-  <si>
-    <t>${R.city}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t>${e.name}</t>
+  </si>
+  <si>
+    <t>${e.buGroup}</t>
+  </si>
+  <si>
+    <t>${e.payment}</t>
+  </si>
+  <si>
+    <t>R{name}</t>
+  </si>
+  <si>
+    <t>R{salary}</t>
+  </si>
+  <si>
+    <t>R{bu=BU}</t>
   </si>
   <si>
     <t>Zeilenbeschriftungen</t>
@@ -112,14 +153,17 @@
     <t>Gesamtergebnis</t>
   </si>
   <si>
-    <t>Anzahl von ${R.city}</t>
+    <t>Summe von R{salary}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +183,19 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,16 +220,20 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -186,17 +247,20 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Marcus Warm" refreshedDate="43741.829868981484" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{CD93B525-49FA-4E45-9644-49573723BC85}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Marcus Warm" refreshedDate="43857.556056828704" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{6A444B79-B34E-4B42-BD11-DF10B7A49F81}">
   <cacheSource type="worksheet">
-    <worksheetSource name="Tabelle1"/>
+    <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="2">
-    <cacheField name="${R.name}" numFmtId="0">
+  <cacheFields count="3">
+    <cacheField name="R{name}" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="R{bu=BU}" numFmtId="0">
       <sharedItems count="1">
-        <s v="${a.name}"/>
+        <s v="${e.buGroup}"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="${R.city}" numFmtId="0">
+    <cacheField name="R{salary}" numFmtId="164">
       <sharedItems/>
     </cacheField>
   </cacheFields>
@@ -211,16 +275,18 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
+    <s v="${e.name}"/>
     <x v="0"/>
-    <s v="${a.city}"/>
+    <s v="${e.payment}"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FE2C7FC0-28D8-464F-ADF7-A6D274C9C78E}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="C6:D8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9CB630A2-C88E-490A-90D7-3505FA002C54}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="C7:D9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="2">
         <item x="0"/>
@@ -230,7 +296,7 @@
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="0"/>
+    <field x="1"/>
   </rowFields>
   <rowItems count="2">
     <i>
@@ -244,7 +310,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Anzahl von ${R.city}" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Summe von R{salary}" fld="2" baseField="1" baseItem="0" numFmtId="164"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -259,11 +325,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C549F59-52AB-4BA5-A571-E25246ABF2AC}" name="Tabelle1" displayName="Tabelle1" ref="A1:B2" totalsRowShown="0">
-  <autoFilter ref="A1:B2" xr:uid="{BF05D0DD-786D-4509-93BB-F3AC158597B0}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{22FBD708-BBDE-4E35-B964-31DB33E08447}" name="${R.name}"/>
-    <tableColumn id="2" xr3:uid="{2169619C-E3C1-48A4-9FB6-A9AF6EA4A890}" name="${R.city}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A8F40B23-2751-4BFF-9A7E-E5258CDD8C24}" name="Table1" displayName="Table1" ref="A1:C2" totalsRowShown="0">
+  <autoFilter ref="A1:C2" xr:uid="{EE13084A-DBE2-424E-8ED9-F7ED27663C92}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{2D231B85-BDE8-4857-8074-54E94611A4C8}" name="R{name}"/>
+    <tableColumn id="2" xr3:uid="{877127D5-7ABE-4EB5-ABA8-C3B78A4E6B1E}" name="R{bu=BU}"/>
+    <tableColumn id="3" xr3:uid="{B67BC07F-EAE4-4701-9E1E-2907E6BD2689}" name="R{salary}" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -565,33 +632,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252A1F08-9B07-4B6A-9E84-D58C1BE989FC}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF88F92-4DB7-4B7A-AA96-8555769868D6}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -604,44 +678,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD70500-13AD-411C-AE36-2E97871CC6F6}">
-  <dimension ref="C6:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDECE3BC-E0DB-454D-B2FD-9279283FBD48}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>